<commit_message>
new elements added to SF and to spectra colors
</commit_message>
<xml_diff>
--- a/configuration/Sensitivity_Factors.xlsx
+++ b/configuration/Sensitivity_Factors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/XPS/XPS_Library/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cassberk/code/xps_peakfit/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71E5E05-35E9-4244-8896-C81212BB5510}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6048DB13-9DD7-134E-B076-9C76B77B5ABB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11940" yWindow="3700" windowWidth="25220" windowHeight="15220" xr2:uid="{C3213E70-0AAA-4401-8FDE-CED959B0E68A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>element</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Mo3d</t>
+  </si>
+  <si>
+    <t>Cr2p</t>
+  </si>
+  <si>
+    <t>Au4f</t>
   </si>
 </sst>
 </file>
@@ -425,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14BA472B-722E-4D10-ADF9-A526FA110BEB}">
   <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -606,6 +612,12 @@
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <v>11.765000000000001</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -898,6 +910,12 @@
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>14</v>
+      </c>
+      <c r="C80">
+        <v>20.734999999999999</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>